<commit_message>
Agregando graficas en el excel y la seccion de banxico
</commit_message>
<xml_diff>
--- a/pruebas/banxico-muestra-5claves.xlsx
+++ b/pruebas/banxico-muestra-5claves.xlsx
@@ -443,35 +443,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SF68616</t>
+          <t>SF64057</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SF325177</t>
+          <t>SF289805</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SF102370</t>
+          <t>SF128322</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SF310365</t>
+          <t>SF26908</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SF69297</t>
+          <t>SF73266</t>
         </is>
       </c>
     </row>

</xml_diff>